<commit_message>
comments added in household.py
</commit_message>
<xml_diff>
--- a/data/input_behavior/BehaviorScenario_Activity_Location.xlsx
+++ b/data/input_behavior/BehaviorScenario_Activity_Location.xlsx
@@ -403,7 +403,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -425,7 +425,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -441,7 +441,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -449,7 +449,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -457,7 +457,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -465,7 +465,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -473,7 +473,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -481,7 +481,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -489,7 +489,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -497,7 +497,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -521,7 +521,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -545,7 +545,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -562,15 +562,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101001383FD7952F44C4AA66F138C1496F932" ma:contentTypeVersion="8" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7a7714bb7e300047a743d6d70b64e471">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ed526690-1b82-4476-9598-c0eeafad58f9" xmlns:ns3="f971c2dd-4979-4752-97a1-eb062e2c22bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bed4c5aeb37c911367c1d98fc4032831" ns2:_="" ns3:_="">
     <xsd:import namespace="ed526690-1b82-4476-9598-c0eeafad58f9"/>
@@ -747,6 +738,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -759,14 +759,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0A26C5C-5A56-4A7C-BB76-118367EE6868}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{802C89E8-F215-4186-8D21-AC5D8A84179F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -785,6 +777,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0A26C5C-5A56-4A7C-BB76-118367EE6868}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96B46992-9108-4E60-AE8D-D8BF3FC36C50}">
   <ds:schemaRefs>

</xml_diff>